<commit_message>
Added edits to day3 day 4 and day7
</commit_message>
<xml_diff>
--- a/Day3/Self-harm dataset.xlsx
+++ b/Day3/Self-harm dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dg519/Documents/Computational-Methods-for-the-Brain-Sciences/Day3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B2C1D-82F8-E446-85F4-9FD36D5D6B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330FB515-FF6D-D94C-8D39-7744876CDDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{5F4A759F-8B9C-2D49-BC90-6443B663A24E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{5F4A759F-8B9C-2D49-BC90-6443B663A24E}"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Harm 1-way" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B91169B-4B92-7E4E-8E6E-1805117D7197}">
   <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="I137" sqref="I137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5621,7 +5621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E488F06C-EAFA-CC4D-A261-C7F57337DC40}">
   <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A104" sqref="A104:A205"/>
     </sheetView>
   </sheetViews>

</xml_diff>